<commit_message>
First commit from feature branch
</commit_message>
<xml_diff>
--- a/Test1.xlsx
+++ b/Test1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523D9DF0-F11F-40EC-A9A2-B6A03FE4B9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9365C9FC-2C5B-4F8C-A7FB-6B2B81D501CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -345,10 +345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:C7"/>
+  <dimension ref="B4:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -363,6 +363,11 @@
         <v>123</v>
       </c>
     </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>456</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>